<commit_message>
write 'Anwesenheitsliste' for Events
</commit_message>
<xml_diff>
--- a/datamanagement-service/src/test/resources/out/Anwesenheitsliste_pro_Veranstaltung.xlsx
+++ b/datamanagement-service/src/test/resources/out/Anwesenheitsliste_pro_Veranstaltung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>Anwesenheitsliste</t>
   </si>
@@ -37,6 +37,24 @@
     <t>Anwesend?</t>
   </si>
   <si>
+    <t>GammaStrahl</t>
+  </si>
+  <si>
+    <t>Mustermann</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>BetaTest</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
     <t>AlphaCut</t>
   </si>
   <si>
@@ -52,24 +70,6 @@
     <t>Peter</t>
   </si>
   <si>
-    <t>BetaTest</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>GammaStrahl</t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>DeltaX</t>
   </si>
   <si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>9:50 – 10:35</t>
+  </si>
+  <si>
+    <t>10:35 – 11:20</t>
   </si>
   <si>
     <t>Company 2</t>
@@ -188,7 +191,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
   </cols>
@@ -247,31 +250,31 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>16</v>
@@ -315,41 +318,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="10" t="s">
+    <row r="17">
+      <c r="A17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="10"/>
+      <c r="D21" s="10"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -376,7 +401,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
   </cols>
@@ -392,7 +417,7 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -435,31 +460,31 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>16</v>
@@ -481,10 +506,32 @@
       </c>
       <c r="D10" s="10"/>
     </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
+    <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>

</xml_diff>